<commit_message>
Added new spreadsheet to fill ingredients with added new csv to start from when cleaning next time
</commit_message>
<xml_diff>
--- a/RecipeIngredients.xlsx
+++ b/RecipeIngredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BirdBoxTreats\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9456AD86-59EF-408C-BBD7-6841EB297254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DB56EA-8E41-48AD-ACC9-64886CFDBE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="900" windowWidth="57600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -987,8 +987,8 @@
   <dimension ref="A1:BP103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y50" sqref="Y50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>